<commit_message>
bom update; pc feup commit
</commit_message>
<xml_diff>
--- a/2. Hardware PCB/REV_4.0/BOM GERAL/BOM_REV4.xlsx
+++ b/2. Hardware PCB/REV_4.0/BOM GERAL/BOM_REV4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="408">
   <si>
     <t>Comment</t>
   </si>
@@ -1238,6 +1238,12 @@
   </si>
   <si>
     <t>R 0018 3W 6432 1%</t>
+  </si>
+  <si>
+    <t>71-WSHP2818R0400FEA</t>
+  </si>
+  <si>
+    <t>R 0040 10W 7146 1%</t>
   </si>
 </sst>
 </file>
@@ -2091,6 +2097,971 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2540,11 +3511,7 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2563,9 +3530,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2582,6 +3546,13 @@
         <scheme val="none"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2617,971 +3588,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3596,28 +3602,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table223" displayName="Table223" ref="A1:N49" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32" totalsRowDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table223" displayName="Table223" ref="A1:N49" totalsRowCount="1" headerRowDxfId="67" dataDxfId="65" totalsRowDxfId="63" headerRowBorderDxfId="66" tableBorderDxfId="64" totalsRowBorderDxfId="62">
   <autoFilter ref="A1:N48"/>
   <sortState ref="A2:O54">
     <sortCondition ref="A1:A54"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Comment" dataDxfId="27" totalsRowDxfId="13"/>
-    <tableColumn id="2" name="Description" dataDxfId="26" totalsRowDxfId="12"/>
-    <tableColumn id="3" name="Designator" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="4" name="Footprint" dataDxfId="24" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="LibRef" dataDxfId="23" totalsRowDxfId="9"/>
-    <tableColumn id="6" name="Quantity" dataDxfId="22" totalsRowDxfId="8"/>
-    <tableColumn id="7" name="Board" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="8" name="RS VPN" dataDxfId="20" totalsRowDxfId="6"/>
-    <tableColumn id="9" name="Farnell VPN" dataDxfId="19" totalsRowDxfId="5"/>
-    <tableColumn id="10" name="Mouser VPN" dataDxfId="18" totalsRowDxfId="4"/>
-    <tableColumn id="14" name="encomendar" dataDxfId="17" totalsRowDxfId="3">
+    <tableColumn id="1" name="Comment" dataDxfId="61" totalsRowDxfId="13"/>
+    <tableColumn id="2" name="Description" dataDxfId="60" totalsRowDxfId="12"/>
+    <tableColumn id="3" name="Designator" dataDxfId="59" totalsRowDxfId="11"/>
+    <tableColumn id="4" name="Footprint" dataDxfId="58" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="LibRef" dataDxfId="57" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Quantity" dataDxfId="56" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Board" dataDxfId="55" totalsRowDxfId="7"/>
+    <tableColumn id="8" name="RS VPN" dataDxfId="54" totalsRowDxfId="6"/>
+    <tableColumn id="9" name="Farnell VPN" dataDxfId="53" totalsRowDxfId="5"/>
+    <tableColumn id="10" name="Mouser VPN" dataDxfId="52" totalsRowDxfId="4"/>
+    <tableColumn id="14" name="encomendar" dataDxfId="51" totalsRowDxfId="3">
       <calculatedColumnFormula>Table223[[#This Row],[Quantity]]*5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="PCDIGA VPN" dataDxfId="16" totalsRowDxfId="2"/>
-    <tableColumn id="11" name="price" totalsRowLabel="TOTAL" dataDxfId="15" totalsRowDxfId="1"/>
-    <tableColumn id="12" name="price REV4" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="0">
+    <tableColumn id="13" name="PCDIGA VPN" dataDxfId="50" totalsRowDxfId="2"/>
+    <tableColumn id="11" name="price" totalsRowLabel="TOTAL" dataDxfId="49" totalsRowDxfId="1"/>
+    <tableColumn id="12" name="price REV4" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="0">
       <calculatedColumnFormula>Table223[[#This Row],[encomendar]]*Table223[[#This Row],[price]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table223[price REV4])</totalsRowFormula>
     </tableColumn>
@@ -3627,28 +3633,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:N86" totalsRowCount="1" headerRowDxfId="67" dataDxfId="66" totalsRowDxfId="65" headerRowBorderDxfId="63" tableBorderDxfId="64" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:N86" totalsRowCount="1" headerRowDxfId="47" dataDxfId="45" totalsRowDxfId="43" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="42">
   <autoFilter ref="A1:N85"/>
   <sortState ref="A2:N85">
     <sortCondition ref="K1:K85"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="Comment" dataDxfId="61" totalsRowDxfId="47"/>
-    <tableColumn id="2" name="Description" dataDxfId="60" totalsRowDxfId="46"/>
-    <tableColumn id="3" name="Designator" dataDxfId="59" totalsRowDxfId="45"/>
-    <tableColumn id="4" name="Footprint" dataDxfId="58" totalsRowDxfId="44"/>
-    <tableColumn id="5" name="LibRef" dataDxfId="57" totalsRowDxfId="43"/>
-    <tableColumn id="6" name="Quantity" dataDxfId="56" totalsRowDxfId="42"/>
-    <tableColumn id="7" name="Board" dataDxfId="55" totalsRowDxfId="41"/>
-    <tableColumn id="8" name="RS VPN" dataDxfId="54" totalsRowDxfId="40"/>
-    <tableColumn id="9" name="Farnell VPN" dataDxfId="53" totalsRowDxfId="39"/>
-    <tableColumn id="10" name="Mouser VPN" dataDxfId="52" totalsRowDxfId="38"/>
-    <tableColumn id="14" name="encomendar" dataDxfId="48" totalsRowDxfId="37">
+    <tableColumn id="1" name="Comment" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" name="Description" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="3" name="Designator" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Footprint" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="5" name="LibRef" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="6" name="Quantity" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="7" name="Board" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="8" name="RS VPN" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="9" name="Farnell VPN" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="10" name="Mouser VPN" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="14" name="encomendar" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>Table22[[#This Row],[Quantity]]*5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="PCDIGA VPN" dataDxfId="51" totalsRowDxfId="36"/>
-    <tableColumn id="11" name="price" totalsRowLabel="TOTAL" dataDxfId="50" totalsRowDxfId="35"/>
-    <tableColumn id="12" name="price total" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="34">
+    <tableColumn id="13" name="PCDIGA VPN" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="11" name="price" totalsRowLabel="TOTAL" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="12" name="price total" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>Table22[[#This Row],[price]]*Table22[[#This Row],[Quantity]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table22[price total])</totalsRowFormula>
     </tableColumn>
@@ -3925,9 +3931,9 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S35" sqref="S35"/>
+      <selection pane="topRight" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5236,7 +5242,7 @@
     </row>
     <row r="32" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>118</v>
+        <v>407</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>93</v>
@@ -5257,11 +5263,9 @@
         <v>255</v>
       </c>
       <c r="H32" s="9"/>
-      <c r="I32" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="I32" s="3"/>
       <c r="J32" s="3" t="s">
-        <v>6</v>
+        <v>406</v>
       </c>
       <c r="K32" s="3">
         <v>20</v>
@@ -5269,12 +5273,12 @@
       <c r="L32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M32" s="17" t="s">
-        <v>285</v>
+      <c r="M32" s="17">
+        <v>1.57</v>
       </c>
       <c r="N32" s="14">
         <f>Table223[[#This Row],[encomendar]]*Table223[[#This Row],[price]]</f>
-        <v>5.42</v>
+        <v>31.400000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -5952,7 +5956,7 @@
       </c>
       <c r="N49" s="26">
         <f>SUM(Table223[price REV4])</f>
-        <v>993.22700000000032</v>
+        <v>1019.2070000000003</v>
       </c>
     </row>
   </sheetData>
@@ -6425,7 +6429,7 @@
         <v>0.45899999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>248</v>
       </c>
@@ -6583,7 +6587,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>370</v>
       </c>
@@ -6616,7 +6620,7 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>246</v>
       </c>
@@ -6659,7 +6663,7 @@
         <v>0.8879999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>357</v>
       </c>
@@ -6778,7 +6782,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="33" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>125</v>
       </c>
@@ -6821,7 +6825,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="54" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>242</v>
       </c>
@@ -7102,7 +7106,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>226</v>
       </c>
@@ -7188,7 +7192,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="24"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -7250,7 +7254,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>264</v>
       </c>
@@ -7464,7 +7468,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>186</v>
       </c>
@@ -7594,7 +7598,7 @@
         <v>14.628</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>158</v>
       </c>
@@ -7676,7 +7680,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>362</v>
       </c>
@@ -7880,7 +7884,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
         <v>131</v>
       </c>
@@ -8078,7 +8082,7 @@
         <v>0.111</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="54" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>268</v>
       </c>
@@ -8122,7 +8126,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>136</v>
       </c>
@@ -8250,7 +8254,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>173</v>
       </c>
@@ -8326,7 +8330,7 @@
         <v>5.0599999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
         <v>363</v>
       </c>
@@ -8402,7 +8406,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>132</v>
       </c>
@@ -8445,7 +8449,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
         <v>368</v>
       </c>
@@ -8482,7 +8486,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="54" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
         <v>127</v>
       </c>
@@ -8614,7 +8618,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>192</v>
       </c>
@@ -8700,7 +8704,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>118</v>
       </c>
@@ -8830,7 +8834,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>221</v>
       </c>
@@ -8874,7 +8878,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>263</v>
       </c>
@@ -9300,7 +9304,7 @@
         <v>3.726</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>157</v>
       </c>
@@ -9344,7 +9348,7 @@
         <v>4.968</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="31" t="s">
         <v>157</v>
       </c>
@@ -9386,7 +9390,7 @@
         <v>4.968</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="54" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>259</v>
       </c>
@@ -9430,7 +9434,7 @@
         <v>14.22</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>216</v>
       </c>
@@ -9567,11 +9571,11 @@
         <v>4.5</v>
       </c>
       <c r="G94" s="39">
-        <f>M94*5</f>
+        <f t="shared" ref="G94:H97" si="0">M94*5</f>
         <v>94.564999999999998</v>
       </c>
       <c r="H94" s="39">
-        <f>N94*5</f>
+        <f t="shared" si="0"/>
         <v>266.82500000000005</v>
       </c>
       <c r="I94" s="39">
@@ -9606,11 +9610,11 @@
         <v>4.5</v>
       </c>
       <c r="G95" s="39">
-        <f>M95*5</f>
+        <f t="shared" si="0"/>
         <v>45.335000000000001</v>
       </c>
       <c r="H95" s="39">
-        <f>N95*5</f>
+        <f t="shared" si="0"/>
         <v>221.375</v>
       </c>
       <c r="I95" s="39">
@@ -9642,11 +9646,11 @@
         <v>4.5</v>
       </c>
       <c r="G96" s="39">
-        <f>M96*5</f>
+        <f t="shared" si="0"/>
         <v>141.68999999999997</v>
       </c>
       <c r="H96" s="39">
-        <f>N96*5</f>
+        <f t="shared" si="0"/>
         <v>146.01</v>
       </c>
       <c r="I96" s="39">
@@ -9678,11 +9682,11 @@
         <v>4.5</v>
       </c>
       <c r="G97" s="39">
-        <f>M97*5</f>
+        <f t="shared" si="0"/>
         <v>59.534999999999997</v>
       </c>
       <c r="H97" s="39">
-        <f>N97*5</f>
+        <f t="shared" si="0"/>
         <v>73.08</v>
       </c>
       <c r="I97" s="39">

</xml_diff>